<commit_message>
reconciled data with card text
still kludge fix for maximum carnage
problem with epic masterminds
</commit_message>
<xml_diff>
--- a/data/henchmen.xlsx
+++ b/data/henchmen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="360" windowWidth="28515" windowHeight="12315" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="360" windowWidth="28515" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
     <t>Set</t>
   </si>
   <si>
-    <t>Spider-infected</t>
-  </si>
-  <si>
     <t>Doombot Legion</t>
   </si>
   <si>
@@ -41,9 +38,6 @@
     <t>Ghost Racers</t>
   </si>
   <si>
-    <t>M.O.D.O.K.S.</t>
-  </si>
-  <si>
     <t>Sentinel</t>
   </si>
   <si>
@@ -65,12 +59,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>Multiple Men</t>
-  </si>
-  <si>
-    <t>SHIELD Assault Squad</t>
-  </si>
-  <si>
     <t>Cape-Killers</t>
   </si>
   <si>
@@ -83,12 +71,6 @@
     <t>Sapien League</t>
   </si>
   <si>
-    <t>Shi'Ar Death Commando's</t>
-  </si>
-  <si>
-    <t>Shi'Ar Patrol Craft</t>
-  </si>
-  <si>
     <t>The Brood</t>
   </si>
   <si>
@@ -221,13 +203,31 @@
     <t>Zero, the Ice Blast</t>
   </si>
   <si>
-    <t>Hydra Base</t>
-  </si>
-  <si>
     <t>Asgardian Warriors</t>
   </si>
   <si>
     <t>Henchmen card name (if separate names)</t>
+  </si>
+  <si>
+    <t>HYDRA Base</t>
+  </si>
+  <si>
+    <t>M.O.D.O.K.s</t>
+  </si>
+  <si>
+    <t>Multiple Man</t>
+  </si>
+  <si>
+    <t>Shi'ar Patrol Craft</t>
+  </si>
+  <si>
+    <t>Shi'ar Death Commandos</t>
+  </si>
+  <si>
+    <t>S.H.I.E.L.D. Assault Squad</t>
+  </si>
+  <si>
+    <t>Spider-Infected</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,46 +596,46 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -646,13 +646,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -669,13 +669,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -686,13 +686,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -700,13 +700,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -717,13 +717,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -737,13 +737,13 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -754,13 +754,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -768,13 +768,13 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -782,13 +782,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -796,57 +796,57 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -857,13 +857,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -874,13 +874,13 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -891,13 +891,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -906,13 +906,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -926,13 +926,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -943,13 +943,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -960,24 +960,24 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -988,13 +988,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C25">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1011,13 +1011,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1034,13 +1034,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C27">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1051,13 +1051,13 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1071,13 +1071,13 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -1085,30 +1085,30 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1119,44 +1119,44 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
         <v>54</v>
       </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1170,44 +1170,44 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1218,16 +1218,16 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -1235,27 +1235,27 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C40">
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1273,7 +1273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1288,15 +1288,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1304,63 +1304,63 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add into the cosmos
no card text or tabletop simulator support yet
</commit_message>
<xml_diff>
--- a/data/henchmen.xlsx
+++ b/data/henchmen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -228,6 +228,21 @@
   </si>
   <si>
     <t>Spider-Infected</t>
+  </si>
+  <si>
+    <t>Sidera Maris, Bridge Builders</t>
+  </si>
+  <si>
+    <t>ITC</t>
+  </si>
+  <si>
+    <t>Universal Church of Truth</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>required shards</t>
   </si>
 </sst>
 </file>
@@ -569,10 +584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -625,7 +641,9 @@
       <c r="K1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
@@ -1131,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1145,7 +1163,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1168,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1182,7 +1200,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1196,7 +1214,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1216,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1233,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -1247,7 +1265,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -1262,6 +1280,37 @@
       </c>
       <c r="J40">
         <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="L42" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
villains and henchmen tags
</commit_message>
<xml_diff>
--- a/data/henchmen.xlsx
+++ b/data/henchmen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>1 2</t>
+  </si>
+  <si>
+    <t>BP</t>
   </si>
 </sst>
 </file>
@@ -722,11 +725,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -734,20 +737,21 @@
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,664 +762,751 @@
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>78</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>80</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
         <v>88</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
         <v>78</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
         <v>78</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
         <v>103</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>65</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
         <v>103</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
         <v>80</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
         <v>88</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
         <v>103</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>80</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>80</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>108</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>62</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>108</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>66</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
         <v>13</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
         <v>108</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>69</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
         <v>13</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
         <v>108</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="C18">
         <v>10</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
         <v>31</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="L18" t="s">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
         <v>85</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="L19" t="s">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="M19" t="s">
         <v>85</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
         <v>36</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
         <v>113</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>17</v>
       </c>
       <c r="C21">
         <v>10</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
         <v>36</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
         <v>113</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>68</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
         <v>36</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
         <v>113</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>67</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
         <v>36</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>113</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
         <v>113</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>41</v>
       </c>
       <c r="C25">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
         <v>42</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
       <c r="F25">
         <v>1</v>
       </c>
-      <c r="J25">
+      <c r="G25">
         <v>1</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
         <v>118</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>43</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
         <v>42</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="J26">
+      <c r="G26">
         <v>1</v>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
         <v>118</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>44</v>
       </c>
       <c r="C27">
         <v>10</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
         <v>42</v>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="L27" t="s">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
         <v>118</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>45</v>
       </c>
       <c r="C28">
         <v>10</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
         <v>46</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
       <c r="F28">
         <v>1</v>
       </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
         <v>78</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>47</v>
       </c>
       <c r="C29">
         <v>10</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
         <v>46</v>
       </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29" t="s">
         <v>78</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1425,17 +1516,20 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
         <v>52</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>91</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1445,23 +1539,26 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
         <v>52</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
       <c r="F31">
         <v>1</v>
       </c>
-      <c r="L31" t="s">
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
         <v>91</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1471,17 +1568,20 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
         <v>52</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>91</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1491,17 +1591,20 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
         <v>52</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>91</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1511,26 +1614,29 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
         <v>52</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
       <c r="F34">
         <v>1</v>
       </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34" t="s">
         <v>91</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1540,17 +1646,20 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
         <v>52</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>91</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1560,17 +1669,20 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
         <v>52</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>91</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1580,23 +1692,26 @@
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
         <v>52</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
         <v>91</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1606,20 +1721,23 @@
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
         <v>52</v>
       </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
-      <c r="L38" t="s">
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="s">
         <v>91</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -1629,79 +1747,91 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
         <v>52</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>91</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>64</v>
       </c>
       <c r="C40">
         <v>10</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
         <v>52</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="M40" t="s">
         <v>91</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>71</v>
       </c>
       <c r="C41">
         <v>10</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
         <v>72</v>
       </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="L41" t="s">
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="M41" t="s">
         <v>117</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>73</v>
       </c>
       <c r="C42">
         <v>10</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
         <v>72</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="L42" t="s">
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="M42" t="s">
         <v>117</v>
       </c>
-      <c r="M42" t="s">
+      <c r="N42" t="s">
         <v>116</v>
       </c>
-      <c r="N42" t="s">
+      <c r="O42" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add MC and DRS
add data for new expansions
start scripting them (untested)
</commit_message>
<xml_diff>
--- a/data/henchmen.xlsx
+++ b/data/henchmen.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -384,6 +384,21 @@
   </si>
   <si>
     <t>BP</t>
+  </si>
+  <si>
+    <t>Mr. Sinister Clones</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>Sentinel Squad O*N*F*</t>
+  </si>
+  <si>
+    <t>mc2,jpg</t>
+  </si>
+  <si>
+    <t>mc2,pjpg</t>
   </si>
 </sst>
 </file>
@@ -725,11 +740,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1835,6 +1850,52 @@
         <v>75</v>
       </c>
     </row>
+    <row r="43" spans="1:15">
+      <c r="A43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>124</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="M43" t="s">
+        <v>126</v>
+      </c>
+      <c r="N43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="M44" t="s">
+        <v>127</v>
+      </c>
+      <c r="N44" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>